<commit_message>
modify the test number of alber
</commit_message>
<xml_diff>
--- a/DatasetDescription.xlsx
+++ b/DatasetDescription.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="6680" yWindow="3340" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,11 +826,11 @@
         <v>7</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1">
-        <v>283493.33333333331</v>
-      </c>
-      <c r="H11" s="1">
-        <v>141746.66666666666</v>
+      <c r="G11" s="3">
+        <v>284910</v>
+      </c>
+      <c r="H11" s="3">
+        <v>140330</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>13</v>

</xml_diff>